<commit_message>
added graph for disparity within the spreadsheet
</commit_message>
<xml_diff>
--- a/Repository-OWL_cv3/Data/distance_tests/Disparity/Combined tests.xlsx
+++ b/Repository-OWL_cv3/Data/distance_tests/Disparity/Combined tests.xlsx
@@ -1,24 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10523"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0E9D6A-F3DB-468F-A74E-84D3E7FF6306}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A08F86F-7D04-3444-A2B1-ACBA41780284}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -98,6 +93,2229 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Calculated</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> distance against measured distance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>test 1 dist mm</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>44.380800000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84.42</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>127.11240000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>163.53360000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>192.96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>212.49720000000002</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>239.51160000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>269.66160000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>291.85199999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>309.45960000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>325.8612</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>339.36840000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>358.42320000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>374.3424</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>397.01520000000005</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>409.07520000000005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>417.51720000000006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>431.98920000000004</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>446.22</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>454.42080000000004</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>466.96320000000003</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>476.12880000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>486.25920000000008</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>494.21880000000004</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>501.21360000000004</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>509.4144</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>518.09760000000006</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>525.0924</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>533.53440000000001</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>537.15240000000006</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>550.9008</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>551.14200000000005</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>556.93080000000009</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A9B3-0C45-89FC-A7B387927ABB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>test 2 dist mm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$H$2:$H$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>116.0172</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>150.26760000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>169.32239999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>185.24160000000003</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>209.36160000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>233.48160000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>255.18960000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>277.13880000000006</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>290.16360000000003</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>310.1832</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>328.51440000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>358.6644</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>375.30720000000008</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>386.64360000000005</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>404.73360000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>406.90440000000007</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>419.92920000000004</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>436.08960000000002</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>447.66720000000004</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>458.76240000000001</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>466.23960000000005</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>481.91760000000005</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>496.87200000000007</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>501.93720000000002</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>517.37400000000002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>531.60480000000007</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>537.39359999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>536.18759999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>543.18240000000003</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>546.55920000000003</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>554.27760000000012</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>558.13679999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>567.78480000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000022-A9B3-0C45-89FC-A7B387927ABB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>test 3 dist mm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>70.1892</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>99.615600000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>136.76</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>166.91</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>182.34700000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>223.11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>239.27</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>258.32499999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>281.72199999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>299.57</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>355.28800000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>377.23700000000002</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>378.44299999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>397.01499999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>408.59300000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>426.2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>437.53699999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>454.66199999999998</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>469.61599999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>453.93799999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>478.541</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>487.46499999999997</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>492.53</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>499.04300000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>506.279</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>543.42399999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>525.09199999999998</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>527.02200000000005</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>541.01199999999994</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>541.01199999999994</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>570.43799999999999</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>579.12099999999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>583.22199999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000023-A9B3-0C45-89FC-A7B387927ABB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>test 4 dist mm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$J$2:$J$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="33"/>
+                <c:pt idx="0">
+                  <c:v>112.158</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>149.54400000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>180.41800000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>204.779</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>221.18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>221.18</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>273.52100000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>288.47500000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>309.21800000000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>337.43900000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>358.18200000000002</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>347.32799999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>370.96600000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>382.30200000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>394.36200000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>409.55799999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>402.80399999999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>432.23</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>412.21100000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>429.577</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>462.38</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>483.36500000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>459.48599999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>500.73099999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>509.41399999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>521.71600000000001</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>528.71</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>536.42899999999997</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>548.00599999999997</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>555.48400000000004</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>562.47799999999995</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>564.89</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>570.67899999999997</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000024-A9B3-0C45-89FC-A7B387927ABB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Actual distance</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="34"/>
+                <c:pt idx="0">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>190</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>220</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>250</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>280</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>290</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000025-A9B3-0C45-89FC-A7B387927ABB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="900565568"/>
+        <c:axId val="900567264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="900565568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Measured</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> Distance mm</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="900567264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="900567264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Calculated Distance mm</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="900565568"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC380FA9-AB8F-DD43-8904-B822584C469E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -365,21 +2583,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18:M19"/>
+    <sheetView tabSelected="1" topLeftCell="M3" workbookViewId="0">
+      <selection activeCell="R22" sqref="R22:R24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5" customWidth="1"/>
-    <col min="5" max="5" width="3.42578125" customWidth="1"/>
-    <col min="6" max="6" width="5.5703125" customWidth="1"/>
-    <col min="7" max="10" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.5" customWidth="1"/>
+    <col min="6" max="6" width="5.5" customWidth="1"/>
+    <col min="7" max="10" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -396,7 +2614,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>180</v>
       </c>
@@ -421,7 +2639,7 @@
         <v>112.158</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>190</v>
       </c>
@@ -436,7 +2654,7 @@
         <v>84.42</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H35" si="1" xml:space="preserve"> ((67 * 3.6)/(1/C3))/1000</f>
+        <f t="shared" ref="H3:H34" si="1" xml:space="preserve"> ((67 * 3.6)/(1/C3))/1000</f>
         <v>150.26760000000002</v>
       </c>
       <c r="I3">
@@ -446,7 +2664,7 @@
         <v>149.54400000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>200</v>
       </c>
@@ -471,7 +2689,7 @@
         <v>180.41800000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>210</v>
       </c>
@@ -496,7 +2714,7 @@
         <v>204.779</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>220</v>
       </c>
@@ -521,7 +2739,7 @@
         <v>221.18</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>230</v>
       </c>
@@ -546,7 +2764,7 @@
         <v>221.18</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>240</v>
       </c>
@@ -571,7 +2789,7 @@
         <v>273.52100000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>250</v>
       </c>
@@ -596,7 +2814,7 @@
         <v>288.47500000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>260</v>
       </c>
@@ -621,7 +2839,7 @@
         <v>309.21800000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>270</v>
       </c>
@@ -646,7 +2864,7 @@
         <v>337.43900000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>280</v>
       </c>
@@ -671,7 +2889,7 @@
         <v>358.18200000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>290</v>
       </c>
@@ -696,7 +2914,7 @@
         <v>347.32799999999997</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>300</v>
       </c>
@@ -721,7 +2939,7 @@
         <v>370.96600000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>310</v>
       </c>
@@ -746,7 +2964,7 @@
         <v>382.30200000000002</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>320</v>
       </c>
@@ -771,7 +2989,7 @@
         <v>394.36200000000002</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>330</v>
       </c>
@@ -796,7 +3014,7 @@
         <v>409.55799999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>340</v>
       </c>
@@ -821,7 +3039,7 @@
         <v>402.80399999999997</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>350</v>
       </c>
@@ -846,7 +3064,7 @@
         <v>432.23</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>360</v>
       </c>
@@ -871,7 +3089,7 @@
         <v>412.21100000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>370</v>
       </c>
@@ -896,7 +3114,7 @@
         <v>429.577</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>380</v>
       </c>
@@ -921,7 +3139,7 @@
         <v>462.38</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>390</v>
       </c>
@@ -946,7 +3164,7 @@
         <v>483.36500000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>400</v>
       </c>
@@ -971,7 +3189,7 @@
         <v>459.48599999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>410</v>
       </c>
@@ -996,7 +3214,7 @@
         <v>500.73099999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>420</v>
       </c>
@@ -1021,7 +3239,7 @@
         <v>509.41399999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>430</v>
       </c>
@@ -1046,7 +3264,7 @@
         <v>521.71600000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>440</v>
       </c>
@@ -1071,7 +3289,7 @@
         <v>528.71</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>450</v>
       </c>
@@ -1096,7 +3314,7 @@
         <v>536.42899999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>460</v>
       </c>
@@ -1121,7 +3339,7 @@
         <v>548.00599999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>470</v>
       </c>
@@ -1146,7 +3364,7 @@
         <v>555.48400000000004</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>480</v>
       </c>
@@ -1171,7 +3389,7 @@
         <v>562.47799999999995</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>490</v>
       </c>
@@ -1196,7 +3414,7 @@
         <v>564.89</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>500</v>
       </c>
@@ -1221,7 +3439,7 @@
         <v>570.67899999999997</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>1</v>
       </c>
@@ -1231,5 +3449,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>